<commit_message>
Link to SKOS-Play! documentation
</commit_message>
<xml_diff>
--- a/codelists/pp_project_fsdfcodes.xlsx
+++ b/codelists/pp_project_fsdfcodes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cox075\dev\AGLDWG\FSDF\codelists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2087D8CD-EDB8-4668-9089-3394F5532D92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09BA927C-F0BF-4449-BD26-B23801602E8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5955" yWindow="3720" windowWidth="31815" windowHeight="17295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11445" yWindow="30" windowWidth="24135" windowHeight="17295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
@@ -20,15 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="92">
   <si>
     <t>uri</t>
   </si>
   <si>
     <t>scheme</t>
-  </si>
-  <si>
-    <t>concept</t>
   </si>
   <si>
     <t>definition@en</t>
@@ -287,6 +284,24 @@
   </si>
   <si>
     <t>https://linked.data.gov.au/def/fsdf/relationship-to-ground</t>
+  </si>
+  <si>
+    <t>Scheme</t>
+  </si>
+  <si>
+    <t>Concept</t>
+  </si>
+  <si>
+    <t>altLabel@en</t>
+  </si>
+  <si>
+    <t>notation</t>
+  </si>
+  <si>
+    <t>http://purl.org/dc/terms/source</t>
+  </si>
+  <si>
+    <t>http://purl.org/dc/terms/subject</t>
   </si>
 </sst>
 </file>
@@ -331,10 +346,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -649,22 +667,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="63.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="255" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" customWidth="1"/>
+    <col min="5" max="5" width="71.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="24" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="47.140625" customWidth="1"/>
+    <col min="9" max="9" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -672,545 +694,558 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
       <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    </row>
+    <row r="5" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+    </row>
+    <row r="6" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>61</v>
       </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="E9" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>67</v>
       </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    </row>
+    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>64</v>
       </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>72</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>69</v>
-      </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>70</v>
-      </c>
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>65</v>
-      </c>
-      <c r="B15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" t="s">
         <v>50</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E17" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E20" t="s">
         <v>46</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E21" t="s">
         <v>38</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E22" t="s">
         <v>34</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E23" t="s">
         <v>44</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E24" t="s">
         <v>48</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E25" t="s">
         <v>40</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E26" t="s">
         <v>36</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B27" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E27" t="s">
         <v>50</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B28" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C28" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E28" t="s">
         <v>42</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B30" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E30" t="s">
         <v>53</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B31" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E31" t="s">
         <v>57</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B32" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C32" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E32" t="s">
         <v>55</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B33" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C33" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E33" t="s">
         <v>42</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>